<commit_message>
FileManager finished Smartphone question intents added Intents organization refactor done
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\644017\PROJECTS\DIALOGFLOW\DialogFlowBackend\Agent\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>synonyms</t>
   </si>
@@ -30,75 +25,15 @@
     <t>smartphoneBrand</t>
   </si>
   <si>
-    <t>['samsung']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LG                </t>
-  </si>
-  <si>
-    <t>['lg']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sony              </t>
-  </si>
-  <si>
-    <t>['sony']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google            </t>
-  </si>
-  <si>
-    <t>['google']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">smartphoneName </t>
-  </si>
-  <si>
-    <t xml:space="preserve">S9                </t>
-  </si>
-  <si>
-    <t>['s9']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S8                </t>
-  </si>
-  <si>
-    <t>['s8']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pixel 2           </t>
-  </si>
-  <si>
-    <t>['pixel 2']</t>
-  </si>
-  <si>
     <t>Xperia XZ1 Compact</t>
   </si>
   <si>
-    <t>['xperia xz1 compact']</t>
-  </si>
-  <si>
     <t>smartphoneRange</t>
   </si>
   <si>
-    <t>['gama baja', 'baja']</t>
-  </si>
-  <si>
-    <t>['gama media', 'media']</t>
-  </si>
-  <si>
-    <t>['gama alta', 'alta']</t>
-  </si>
-  <si>
-    <t>['gama premium', 'premium']</t>
-  </si>
-  <si>
     <t xml:space="preserve">testParameter  </t>
   </si>
   <si>
-    <t>['test', 'testing']</t>
-  </si>
-  <si>
     <t>entity</t>
   </si>
   <si>
@@ -129,19 +64,91 @@
     <t>value</t>
   </si>
   <si>
-    <t>['smartphone', 'phone', 'móvil', 'terminal móvil', 'teléfono', 'smartphones']</t>
-  </si>
-  <si>
     <t>New value</t>
   </si>
   <si>
-    <t>['value']</t>
+    <t>samsung</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>sony</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>s8</t>
+  </si>
+  <si>
+    <t>pixel 2</t>
+  </si>
+  <si>
+    <t>xperia xz1 compact</t>
+  </si>
+  <si>
+    <t>test testing</t>
+  </si>
+  <si>
+    <t>smartphone
+phone
+móvil
+terminal
+móvil
+teléfono
+smartphones</t>
+  </si>
+  <si>
+    <t>gama baja
+baja</t>
+  </si>
+  <si>
+    <t>gama media
+media</t>
+  </si>
+  <si>
+    <t>gama alta
+alta</t>
+  </si>
+  <si>
+    <t>gama premium
+premium</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sony  </t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>smartphoneName</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>el
+cuál
+1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -619,55 +626,61 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,7 +738,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -760,7 +773,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -937,7 +950,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -945,190 +958,220 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.7109375" customWidth="1"/>
     <col min="2" max="2" width="53.7109375" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" customWidth="1"/>
+    <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
+      <c r="B10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding intent exception handler Schema arg for RUN command FileManager fixed for Annotations in user_says excel
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
@@ -10,11 +10,12 @@
     <sheet name="entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>synonyms</t>
   </si>
@@ -31,9 +32,6 @@
     <t>smartphoneRange</t>
   </si>
   <si>
-    <t xml:space="preserve">testParameter  </t>
-  </si>
-  <si>
     <t>entity</t>
   </si>
   <si>
@@ -46,9 +44,6 @@
     <t>Gama premium</t>
   </si>
   <si>
-    <t>Test Value</t>
-  </si>
-  <si>
     <t>Gama alta</t>
   </si>
   <si>
@@ -64,9 +59,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>New value</t>
-  </si>
-  <si>
     <t>samsung</t>
   </si>
   <si>
@@ -91,58 +83,114 @@
     <t>xperia xz1 compact</t>
   </si>
   <si>
-    <t>test testing</t>
+    <t>gama baja
+baja</t>
+  </si>
+  <si>
+    <t>gama media
+media</t>
+  </si>
+  <si>
+    <t>gama alta
+alta</t>
+  </si>
+  <si>
+    <t>gama premium
+premium</t>
+  </si>
+  <si>
+    <t>LG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sony  </t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>smartphoneName</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t>xiaomi</t>
+  </si>
+  <si>
+    <t>huawei</t>
+  </si>
+  <si>
+    <t>apple
+iphone</t>
+  </si>
+  <si>
+    <t>2
+dos</t>
+  </si>
+  <si>
+    <t>3
+tres</t>
+  </si>
+  <si>
+    <t>4
+cuatro</t>
+  </si>
+  <si>
+    <t>5
+cinco</t>
+  </si>
+  <si>
+    <t>6
+seis</t>
+  </si>
+  <si>
+    <t>7
+siete</t>
+  </si>
+  <si>
+    <t>8
+ocho</t>
+  </si>
+  <si>
+    <t>9
+nueve</t>
+  </si>
+  <si>
+    <t>10
+diez</t>
+  </si>
+  <si>
+    <t>es
+el
+cuál
+1
+un
+uno</t>
   </si>
   <si>
     <t>smartphone
 phone
 móvil
-terminal
-móvil
+terminal móvil
 teléfono
-smartphones</t>
-  </si>
-  <si>
-    <t>gama baja
-baja</t>
-  </si>
-  <si>
-    <t>gama media
-media</t>
-  </si>
-  <si>
-    <t>gama alta
-alta</t>
-  </si>
-  <si>
-    <t>gama premium
-premium</t>
-  </si>
-  <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sony  </t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>S8</t>
-  </si>
-  <si>
-    <t>smartphoneName</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>el
-cuál
-1</t>
+smartphones
+moviles
+telefonos</t>
   </si>
 </sst>
 </file>
@@ -632,10 +680,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -687,9 +735,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -950,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -958,10 +1003,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,206 +1017,275 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>22</v>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1">
         <v>4</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="1">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="1">
         <v>9</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="1">
         <v>10</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="2">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>38</v>
+      <c r="C28" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
+    <mergeCell ref="A19:A28"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding AgentSays from Excel functionality. Adding new intent for SmartPhone differences
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -10,12 +10,11 @@
     <sheet name="entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>synonyms</t>
   </si>
@@ -191,6 +190,12 @@
 smartphones
 moviles
 telefonos</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>g6</t>
   </si>
 </sst>
 </file>
@@ -674,13 +679,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -995,7 +1003,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1003,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A10" sqref="A10:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1047,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1050,7 +1058,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1059,7 +1067,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1068,7 +1076,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1104,7 +1112,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1115,7 +1123,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1124,7 +1132,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1133,7 +1141,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1150,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1150,142 +1158,151 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1" t="s">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1" t="s">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="1">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="1">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="1">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1">
         <v>4</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="1">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="1">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1">
         <v>6</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="1">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1">
         <v>7</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="1">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="1">
         <v>8</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="1">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="1">
         <v>9</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="1">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1">
         <v>10</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="A20:A29"/>
     <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A10:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed graphics module Added sp.selected intents
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>synonyms</t>
   </si>
@@ -196,6 +196,17 @@
   </si>
   <si>
     <t>g6</t>
+  </si>
+  <si>
+    <t>6
+plus 6</t>
+  </si>
+  <si>
+    <t>One Plus</t>
+  </si>
+  <si>
+    <t>one plus
+oneplus</t>
   </si>
 </sst>
 </file>
@@ -679,13 +690,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1003,7 +1017,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1011,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A15"/>
+      <selection activeCell="C16" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1061,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1058,7 +1072,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1067,7 +1081,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1076,7 +1090,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1085,7 +1099,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1094,7 +1108,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1103,7 +1117,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1111,198 +1125,216 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="1" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="1" t="s">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1" t="s">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1" t="s">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="1">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="1">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="1">
         <v>4</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="1">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="1">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="1">
         <v>6</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="1">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="1">
         <v>7</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="1">
         <v>8</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="1">
         <v>9</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="1">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="1">
         <v>10</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A20:A29"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A22:A31"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A3:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed intents and schema
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>synonyms</t>
   </si>
@@ -221,6 +221,26 @@
   <si>
     <t>a8
 galaxy a8</t>
+  </si>
+  <si>
+    <t>Redmi Note 4</t>
+  </si>
+  <si>
+    <t>Note 4
+redmi 4
+redmi note 4</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>p 20</t>
+  </si>
+  <si>
+    <t>P20 lite</t>
+  </si>
+  <si>
+    <t>p 20 lite</t>
   </si>
 </sst>
 </file>
@@ -704,13 +724,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1034,7 +1057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1042,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D23:D24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1101,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1089,7 +1112,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1098,7 +1121,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
@@ -1107,7 +1130,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1116,7 +1139,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1125,7 +1148,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1134,7 +1157,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1143,12 +1166,12 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
         <v>53</v>
       </c>
@@ -1157,7 +1180,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1168,7 +1191,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1177,7 +1200,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1186,7 +1209,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1218,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1227,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
@@ -1213,7 +1236,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="4">
         <v>6</v>
       </c>
@@ -1222,7 +1245,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="5" t="s">
         <v>55</v>
       </c>
@@ -1231,7 +1254,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="5" t="s">
         <v>57</v>
       </c>
@@ -1239,142 +1262,169 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1" t="s">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="1" t="s">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="1" t="s">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="28" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="1">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1">
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="1">
         <v>3</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="1">
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1">
         <v>4</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="1">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="1">
         <v>5</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1">
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="1">
         <v>6</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="1">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="1">
         <v>7</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="1">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="1">
         <v>8</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="1">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="1">
         <v>9</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="1">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="1">
         <v>10</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A28:A37"/>
+    <mergeCell ref="A24:A27"/>
     <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A20"/>
+    <mergeCell ref="A12:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed errors for demo. Added eCommerceSelected intent
</commit_message>
<xml_diff>
--- a/Agent/entities.xlsx
+++ b/Agent/entities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>synonyms</t>
   </si>
@@ -241,6 +241,36 @@
   </si>
   <si>
     <t>p 20 lite</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>MediaMarkt</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>GearBest</t>
+  </si>
+  <si>
+    <t>eCommerceName</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>mediamarkt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aliexpres
+ali express
+</t>
+  </si>
+  <si>
+    <t>gearbest
+gear best</t>
   </si>
 </sst>
 </file>
@@ -724,7 +754,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -746,6 +776,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1065,10 +1101,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C50" sqref="C49:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,12 +1455,51 @@
         <v>47</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A28:A37"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A12:A23"/>
+    <mergeCell ref="A38:A41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>